<commit_message>
Updated File path in KeyManager
</commit_message>
<xml_diff>
--- a/src/test/resources/data/jdgroupTA541.xlsx
+++ b/src/test/resources/data/jdgroupTA541.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23628"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D54AD08-249D-466C-9A14-1FB15E018E5A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1FD19F0-B9AD-4F4A-BDD9-90D89343577C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" firstSheet="2" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="evs_SAP_OrderRelated++" sheetId="93" r:id="rId1"/>
@@ -3517,17 +3517,7 @@
     <cellStyle name="Normal 2 2" xfId="4" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
     <cellStyle name="Normal 3" xfId="3" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
   </cellStyles>
-  <dxfs count="149">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="148">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -5607,7 +5597,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2">
-    <cfRule type="duplicateValues" dxfId="96" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="95" priority="1"/>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="A1" location="EVS!A1" display="TCID" xr:uid="{00000000-0004-0000-0B00-000000000000}"/>
@@ -6294,7 +6284,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2">
-    <cfRule type="duplicateValues" dxfId="95" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="94" priority="1"/>
   </conditionalFormatting>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2" xr:uid="{00000000-0002-0000-0E00-000000000000}">
@@ -7511,25 +7501,25 @@
   </sheetData>
   <phoneticPr fontId="8" type="noConversion"/>
   <conditionalFormatting sqref="B12:B15">
-    <cfRule type="duplicateValues" dxfId="94" priority="10"/>
+    <cfRule type="duplicateValues" dxfId="93" priority="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B16">
-    <cfRule type="duplicateValues" dxfId="93" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="92" priority="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A16">
-    <cfRule type="duplicateValues" dxfId="92" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="91" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B29">
-    <cfRule type="duplicateValues" dxfId="91" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="90" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B30:B33">
-    <cfRule type="duplicateValues" dxfId="90" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="89" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B9">
-    <cfRule type="duplicateValues" dxfId="89" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="88" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B8">
-    <cfRule type="duplicateValues" dxfId="88" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="87" priority="1"/>
   </conditionalFormatting>
   <dataValidations count="3">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H16" xr:uid="{00000000-0002-0000-0F00-000000000000}">
@@ -8806,22 +8796,22 @@
   </sheetData>
   <phoneticPr fontId="8" type="noConversion"/>
   <conditionalFormatting sqref="A27">
-    <cfRule type="duplicateValues" dxfId="87" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="86" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B27">
-    <cfRule type="duplicateValues" dxfId="86" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="85" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B28:B31">
-    <cfRule type="duplicateValues" dxfId="85" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="84" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A28:A31">
-    <cfRule type="duplicateValues" dxfId="84" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="83" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B12:B26">
-    <cfRule type="duplicateValues" dxfId="83" priority="65"/>
+    <cfRule type="duplicateValues" dxfId="82" priority="65"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A12:A26">
-    <cfRule type="duplicateValues" dxfId="82" priority="66"/>
+    <cfRule type="duplicateValues" dxfId="81" priority="66"/>
   </conditionalFormatting>
   <dataValidations count="4">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M2:M11 M32" xr:uid="{00000000-0002-0000-1000-000000000000}">
@@ -9141,7 +9131,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2">
-    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="80" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -9353,10 +9343,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:B6">
-    <cfRule type="duplicateValues" dxfId="81" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="79" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B7">
-    <cfRule type="duplicateValues" dxfId="80" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="78" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -9564,10 +9554,10 @@
   </sheetData>
   <phoneticPr fontId="8" type="noConversion"/>
   <conditionalFormatting sqref="B2:B3">
-    <cfRule type="duplicateValues" dxfId="79" priority="67"/>
+    <cfRule type="duplicateValues" dxfId="77" priority="67"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:A3">
-    <cfRule type="duplicateValues" dxfId="78" priority="69"/>
+    <cfRule type="duplicateValues" dxfId="76" priority="69"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -9718,16 +9708,16 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2 B4">
-    <cfRule type="duplicateValues" dxfId="77" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="75" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2 A4">
-    <cfRule type="duplicateValues" dxfId="76" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="74" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3">
-    <cfRule type="duplicateValues" dxfId="75" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="73" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A3">
-    <cfRule type="duplicateValues" dxfId="74" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="72" priority="1"/>
   </conditionalFormatting>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D4" xr:uid="{00000000-0002-0000-1700-000000000000}">
@@ -9943,10 +9933,10 @@
   </sheetData>
   <phoneticPr fontId="8" type="noConversion"/>
   <conditionalFormatting sqref="B2:B3">
-    <cfRule type="duplicateValues" dxfId="73" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="71" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:A3">
-    <cfRule type="duplicateValues" dxfId="72" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="70" priority="1"/>
   </conditionalFormatting>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D3" xr:uid="{00000000-0002-0000-1800-000000000000}">
@@ -10338,22 +10328,22 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:A21">
-    <cfRule type="duplicateValues" dxfId="71" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="69" priority="7"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:B21">
-    <cfRule type="duplicateValues" dxfId="70" priority="8"/>
+    <cfRule type="duplicateValues" dxfId="68" priority="8"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A22">
-    <cfRule type="duplicateValues" dxfId="69" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="67" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B22">
-    <cfRule type="duplicateValues" dxfId="68" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="66" priority="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A23:A26">
-    <cfRule type="duplicateValues" dxfId="67" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="65" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B23:B26">
-    <cfRule type="duplicateValues" dxfId="66" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="64" priority="2"/>
   </conditionalFormatting>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576" xr:uid="{00000000-0002-0000-1900-000000000000}">
@@ -10450,7 +10440,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:B4">
-    <cfRule type="duplicateValues" dxfId="65" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="63" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -10510,10 +10500,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2">
-    <cfRule type="duplicateValues" dxfId="64" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="62" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2">
-    <cfRule type="duplicateValues" dxfId="63" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="61" priority="2"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -10523,7 +10513,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
@@ -10803,10 +10793,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:A3">
-    <cfRule type="duplicateValues" dxfId="62" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="60" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:B3">
-    <cfRule type="duplicateValues" dxfId="61" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="59" priority="2"/>
   </conditionalFormatting>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576" xr:uid="{00000000-0002-0000-1C00-000000000000}">
@@ -10931,10 +10921,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:A3">
-    <cfRule type="duplicateValues" dxfId="60" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="58" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:B3">
-    <cfRule type="duplicateValues" dxfId="59" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="57" priority="2"/>
   </conditionalFormatting>
   <dataValidations count="3">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576" xr:uid="{00000000-0002-0000-1D00-000000000000}">
@@ -11083,10 +11073,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:A3">
-    <cfRule type="duplicateValues" dxfId="58" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="56" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:B3">
-    <cfRule type="duplicateValues" dxfId="57" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="55" priority="2"/>
   </conditionalFormatting>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F1048576" xr:uid="{00000000-0002-0000-1E00-000000000000}">
@@ -11210,10 +11200,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:A3">
-    <cfRule type="duplicateValues" dxfId="56" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="54" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:B3">
-    <cfRule type="duplicateValues" dxfId="55" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="53" priority="2"/>
   </conditionalFormatting>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576" xr:uid="{00000000-0002-0000-1F00-000000000000}">
@@ -11466,10 +11456,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:A3">
-    <cfRule type="duplicateValues" dxfId="54" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="52" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:B3">
-    <cfRule type="duplicateValues" dxfId="53" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="51" priority="2"/>
   </conditionalFormatting>
   <dataValidations count="7">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:I3 Q2:Q3" xr:uid="{00000000-0002-0000-2000-000000000000}">
@@ -11561,10 +11551,10 @@
   </sheetData>
   <phoneticPr fontId="8" type="noConversion"/>
   <conditionalFormatting sqref="A2">
-    <cfRule type="duplicateValues" dxfId="52" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="50" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2">
-    <cfRule type="duplicateValues" dxfId="51" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="49" priority="2"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -11616,10 +11606,10 @@
   </sheetData>
   <phoneticPr fontId="8" type="noConversion"/>
   <conditionalFormatting sqref="A2">
-    <cfRule type="duplicateValues" dxfId="50" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="48" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2">
-    <cfRule type="duplicateValues" dxfId="49" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="47" priority="2"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -12349,22 +12339,22 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A22">
-    <cfRule type="duplicateValues" dxfId="48" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="46" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B22">
-    <cfRule type="duplicateValues" dxfId="47" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="45" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B23:B25">
-    <cfRule type="duplicateValues" dxfId="46" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="44" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A23:A25">
-    <cfRule type="duplicateValues" dxfId="45" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="43" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B8:B21">
-    <cfRule type="duplicateValues" dxfId="44" priority="45"/>
+    <cfRule type="duplicateValues" dxfId="42" priority="45"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A8:A21">
-    <cfRule type="duplicateValues" dxfId="43" priority="47"/>
+    <cfRule type="duplicateValues" dxfId="41" priority="47"/>
   </conditionalFormatting>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Y3:Y10 Q2:Q10" xr:uid="{00000000-0002-0000-2400-000000000000}">
@@ -13025,22 +13015,22 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A22">
-    <cfRule type="duplicateValues" dxfId="42" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="40" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B22">
-    <cfRule type="duplicateValues" dxfId="41" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="39" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B23:B25">
-    <cfRule type="duplicateValues" dxfId="40" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="38" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A23:A25">
-    <cfRule type="duplicateValues" dxfId="39" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="37" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B8:B21">
-    <cfRule type="duplicateValues" dxfId="38" priority="28"/>
+    <cfRule type="duplicateValues" dxfId="36" priority="28"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A8:A21">
-    <cfRule type="duplicateValues" dxfId="37" priority="29"/>
+    <cfRule type="duplicateValues" dxfId="35" priority="29"/>
   </conditionalFormatting>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576 F2:F1048576 H2:H1048576 J2:J1048576 L2:L1048576 N2:O1048576" xr:uid="{00000000-0002-0000-2500-000000000000}">
@@ -13586,10 +13576,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A23:A25">
-    <cfRule type="duplicateValues" dxfId="36" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="34" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B23:B25">
-    <cfRule type="duplicateValues" dxfId="35" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="33" priority="2"/>
   </conditionalFormatting>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576" xr:uid="{00000000-0002-0000-2600-000000000000}">
@@ -14040,7 +14030,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B12:B14">
-    <cfRule type="duplicateValues" dxfId="34" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="32" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -14273,7 +14263,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B13:B15">
-    <cfRule type="duplicateValues" dxfId="33" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="31" priority="1"/>
   </conditionalFormatting>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576" xr:uid="{00000000-0002-0000-2800-000000000000}">
@@ -15140,16 +15130,16 @@
   </sheetData>
   <phoneticPr fontId="8" type="noConversion"/>
   <conditionalFormatting sqref="B10:B12">
-    <cfRule type="duplicateValues" dxfId="32" priority="9"/>
+    <cfRule type="duplicateValues" dxfId="30" priority="9"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B13">
-    <cfRule type="duplicateValues" dxfId="31" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="29" priority="7"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B14:B33">
-    <cfRule type="duplicateValues" dxfId="30" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="28" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A14:A33">
-    <cfRule type="duplicateValues" dxfId="29" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="27" priority="6"/>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="O2" r:id="rId1" xr:uid="{00000000-0004-0000-2900-000000000000}"/>
@@ -15321,16 +15311,16 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:B6">
-    <cfRule type="duplicateValues" dxfId="28" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="26" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:A6">
-    <cfRule type="duplicateValues" dxfId="27" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="25" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B7:B12">
-    <cfRule type="duplicateValues" dxfId="26" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="24" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A7:A12">
-    <cfRule type="duplicateValues" dxfId="25" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="23" priority="2"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -15749,10 +15739,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B11:B13">
-    <cfRule type="duplicateValues" dxfId="24" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="22" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A11:A13">
-    <cfRule type="duplicateValues" dxfId="23" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="21" priority="2"/>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="A1" location="EVS!A1" display="TCID" xr:uid="{00000000-0004-0000-2C00-000000000000}"/>
@@ -16015,7 +16005,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B11:B13">
-    <cfRule type="duplicateValues" dxfId="22" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="20" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -16272,7 +16262,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B13:B15">
-    <cfRule type="duplicateValues" dxfId="21" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="19" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -16500,16 +16490,16 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B12">
-    <cfRule type="duplicateValues" dxfId="20" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="18" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B13">
-    <cfRule type="duplicateValues" dxfId="19" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="17" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B14">
-    <cfRule type="duplicateValues" dxfId="18" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="16" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B8">
-    <cfRule type="duplicateValues" dxfId="17" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="15" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -17257,25 +17247,25 @@
   </sheetData>
   <phoneticPr fontId="8" type="noConversion"/>
   <conditionalFormatting sqref="B33:B35">
-    <cfRule type="duplicateValues" dxfId="148" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="147" priority="7"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A36">
-    <cfRule type="duplicateValues" dxfId="147" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="146" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B36">
-    <cfRule type="duplicateValues" dxfId="146" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="145" priority="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A31:A32">
-    <cfRule type="duplicateValues" dxfId="145" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="144" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B31:B32">
-    <cfRule type="duplicateValues" dxfId="144" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="143" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A37">
-    <cfRule type="duplicateValues" dxfId="143" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="142" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B37">
-    <cfRule type="duplicateValues" dxfId="142" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="141" priority="2"/>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="A1" location="EVS!A1" display="TCID" xr:uid="{00000000-0004-0000-0400-000000000000}"/>
@@ -18170,16 +18160,16 @@
   </sheetData>
   <phoneticPr fontId="8" type="noConversion"/>
   <conditionalFormatting sqref="B13:B16">
-    <cfRule type="duplicateValues" dxfId="16" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="14" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A11:A12">
-    <cfRule type="duplicateValues" dxfId="15" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="13" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B11:B12">
-    <cfRule type="duplicateValues" dxfId="14" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="12" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B19:B21">
-    <cfRule type="duplicateValues" dxfId="13" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="11" priority="1"/>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="F2" r:id="rId1" xr:uid="{00000000-0004-0000-3400-000000000000}"/>
@@ -18384,16 +18374,16 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B9:B12">
-    <cfRule type="duplicateValues" dxfId="12" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="10" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A9:A12">
-    <cfRule type="duplicateValues" dxfId="11" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="9" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B4">
-    <cfRule type="duplicateValues" dxfId="10" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="8" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B5:B7">
-    <cfRule type="duplicateValues" dxfId="9" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="7" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -18490,7 +18480,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:B3">
-    <cfRule type="duplicateValues" dxfId="8" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="6" priority="1"/>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="G2" r:id="rId1" xr:uid="{55122947-C721-424F-895C-6737C39F195B}"/>
@@ -19730,22 +19720,22 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A22">
-    <cfRule type="duplicateValues" dxfId="7" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="5" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B22">
-    <cfRule type="duplicateValues" dxfId="6" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="4" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B23:B25">
-    <cfRule type="duplicateValues" dxfId="5" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="3" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A23:A25">
-    <cfRule type="duplicateValues" dxfId="4" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B5:B21">
-    <cfRule type="duplicateValues" dxfId="3" priority="54"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="54"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A5:A21">
-    <cfRule type="duplicateValues" dxfId="2" priority="56"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="56"/>
   </conditionalFormatting>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J4" xr:uid="{00000000-0002-0000-3C00-000000000000}">
@@ -20704,7 +20694,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C64" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A65" sqref="A65:XFD65"/>
+      <selection pane="bottomRight" activeCell="A66" sqref="A66:XFD66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -24138,121 +24128,121 @@
   </sheetData>
   <phoneticPr fontId="8" type="noConversion"/>
   <conditionalFormatting sqref="B54">
-    <cfRule type="duplicateValues" dxfId="141" priority="49"/>
+    <cfRule type="duplicateValues" dxfId="140" priority="49"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A32">
-    <cfRule type="duplicateValues" dxfId="140" priority="46"/>
+    <cfRule type="duplicateValues" dxfId="139" priority="46"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B32">
-    <cfRule type="duplicateValues" dxfId="139" priority="47"/>
+    <cfRule type="duplicateValues" dxfId="138" priority="47"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B50:B52">
-    <cfRule type="duplicateValues" dxfId="138" priority="45"/>
+    <cfRule type="duplicateValues" dxfId="137" priority="45"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D47">
-    <cfRule type="duplicateValues" dxfId="137" priority="42"/>
+    <cfRule type="duplicateValues" dxfId="136" priority="42"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A53:A54 A2:A31 A33:A49">
-    <cfRule type="duplicateValues" dxfId="136" priority="53"/>
+    <cfRule type="duplicateValues" dxfId="135" priority="53"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D32">
-    <cfRule type="duplicateValues" dxfId="135" priority="41"/>
+    <cfRule type="duplicateValues" dxfId="134" priority="41"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D30">
-    <cfRule type="duplicateValues" dxfId="134" priority="37"/>
+    <cfRule type="duplicateValues" dxfId="133" priority="37"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D31">
-    <cfRule type="duplicateValues" dxfId="133" priority="36"/>
+    <cfRule type="duplicateValues" dxfId="132" priority="36"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D74">
-    <cfRule type="duplicateValues" dxfId="132" priority="35"/>
+    <cfRule type="duplicateValues" dxfId="131" priority="35"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B76">
-    <cfRule type="duplicateValues" dxfId="131" priority="34"/>
+    <cfRule type="duplicateValues" dxfId="130" priority="34"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B77">
-    <cfRule type="duplicateValues" dxfId="130" priority="33"/>
+    <cfRule type="duplicateValues" dxfId="129" priority="33"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B78">
-    <cfRule type="duplicateValues" dxfId="129" priority="32"/>
+    <cfRule type="duplicateValues" dxfId="128" priority="32"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B79">
-    <cfRule type="duplicateValues" dxfId="128" priority="31"/>
+    <cfRule type="duplicateValues" dxfId="127" priority="31"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D58">
-    <cfRule type="duplicateValues" dxfId="127" priority="30"/>
+    <cfRule type="duplicateValues" dxfId="126" priority="30"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D59">
-    <cfRule type="duplicateValues" dxfId="126" priority="29"/>
+    <cfRule type="duplicateValues" dxfId="125" priority="29"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D60">
-    <cfRule type="duplicateValues" dxfId="125" priority="28"/>
+    <cfRule type="duplicateValues" dxfId="124" priority="28"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D61">
-    <cfRule type="duplicateValues" dxfId="124" priority="27"/>
+    <cfRule type="duplicateValues" dxfId="123" priority="27"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D62">
-    <cfRule type="duplicateValues" dxfId="123" priority="26"/>
+    <cfRule type="duplicateValues" dxfId="122" priority="26"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D75">
-    <cfRule type="duplicateValues" dxfId="122" priority="25"/>
+    <cfRule type="duplicateValues" dxfId="121" priority="25"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D76">
-    <cfRule type="duplicateValues" dxfId="121" priority="24"/>
+    <cfRule type="duplicateValues" dxfId="120" priority="24"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D77">
-    <cfRule type="duplicateValues" dxfId="120" priority="23"/>
+    <cfRule type="duplicateValues" dxfId="119" priority="23"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D78">
-    <cfRule type="duplicateValues" dxfId="119" priority="22"/>
+    <cfRule type="duplicateValues" dxfId="118" priority="22"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D79">
-    <cfRule type="duplicateValues" dxfId="118" priority="21"/>
+    <cfRule type="duplicateValues" dxfId="117" priority="21"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B94:B1048576 B81:B84 B33:B49 B1:B31 B55:B75">
-    <cfRule type="duplicateValues" dxfId="117" priority="90"/>
+    <cfRule type="duplicateValues" dxfId="116" priority="90"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D72">
-    <cfRule type="duplicateValues" dxfId="116" priority="20"/>
+    <cfRule type="duplicateValues" dxfId="115" priority="20"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D73">
-    <cfRule type="duplicateValues" dxfId="115" priority="19"/>
+    <cfRule type="duplicateValues" dxfId="114" priority="19"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B85">
-    <cfRule type="duplicateValues" dxfId="114" priority="16"/>
+    <cfRule type="duplicateValues" dxfId="113" priority="16"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B86">
-    <cfRule type="duplicateValues" dxfId="113" priority="15"/>
+    <cfRule type="duplicateValues" dxfId="112" priority="15"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B87">
-    <cfRule type="duplicateValues" dxfId="112" priority="14"/>
+    <cfRule type="duplicateValues" dxfId="111" priority="14"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D87">
-    <cfRule type="duplicateValues" dxfId="111" priority="13"/>
+    <cfRule type="duplicateValues" dxfId="110" priority="13"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B88:B92">
-    <cfRule type="duplicateValues" dxfId="110" priority="12"/>
+    <cfRule type="duplicateValues" dxfId="109" priority="12"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G88:I91">
-    <cfRule type="duplicateValues" dxfId="109" priority="10"/>
+    <cfRule type="duplicateValues" dxfId="108" priority="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B93">
-    <cfRule type="duplicateValues" dxfId="108" priority="9"/>
+    <cfRule type="duplicateValues" dxfId="107" priority="9"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D88:D91">
-    <cfRule type="duplicateValues" dxfId="107" priority="8"/>
+    <cfRule type="duplicateValues" dxfId="106" priority="8"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D93">
-    <cfRule type="duplicateValues" dxfId="106" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="105" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D92">
-    <cfRule type="duplicateValues" dxfId="105" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="104" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G92:G93">
-    <cfRule type="duplicateValues" dxfId="104" priority="95"/>
+    <cfRule type="duplicateValues" dxfId="103" priority="95"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B53">
-    <cfRule type="duplicateValues" dxfId="103" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="102" priority="1"/>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="H3" location="'Login_magento++'!A1" display="Login_magento" xr:uid="{00000000-0004-0000-0600-000000000000}"/>
@@ -24733,11 +24723,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:T9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G9" sqref="G9"/>
+      <selection pane="bottomRight" activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -25088,22 +25078,22 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2">
-    <cfRule type="duplicateValues" dxfId="102" priority="24"/>
+    <cfRule type="duplicateValues" dxfId="101" priority="24"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2">
-    <cfRule type="duplicateValues" dxfId="101" priority="23"/>
+    <cfRule type="duplicateValues" dxfId="100" priority="23"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3:B8">
-    <cfRule type="duplicateValues" dxfId="100" priority="22"/>
+    <cfRule type="duplicateValues" dxfId="99" priority="22"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3:D8">
-    <cfRule type="duplicateValues" dxfId="99" priority="21"/>
+    <cfRule type="duplicateValues" dxfId="98" priority="21"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1">
-    <cfRule type="duplicateValues" dxfId="98" priority="115"/>
+    <cfRule type="duplicateValues" dxfId="97" priority="115"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B9">
-    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="96" priority="1"/>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="G2" location="'evs_ProductSearch++'!A1" display="evs_ProductSearch" xr:uid="{00000000-0004-0000-0700-000000000000}"/>
@@ -25174,6 +25164,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101009E4315169E4449459811E1A2A421A5D2" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="484de8a0a7035cbf3240ac5ef037eda8">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="38ec8e4d-8506-4d8b-b040-96d37469ddf9" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="40b4f8b6fbe630a6badbf346a8d0e64c" ns1:_="" ns2:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -25322,7 +25321,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
@@ -25331,16 +25330,15 @@
 </p:properties>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{525C0858-3CD6-4044-8BEB-39A1DA4B5834}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EED871C4-2A4D-4B74-98A2-587321F60978}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -25359,7 +25357,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D73877E0-ACC9-4E95-9DFE-6B4A6282CC78}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -25374,12 +25372,4 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{525C0858-3CD6-4044-8BEB-39A1DA4B5834}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>